<commit_message>
Homehelp status dates refactoring
</commit_message>
<xml_diff>
--- a/src/JCSGYK/AdminBundle/Resources/public/reports/catering_stats.xlsx
+++ b/src/JCSGYK/AdminBundle/Resources/public/reports/catering_stats.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="2380" yWindow="1340" windowWidth="46380" windowHeight="26420"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>[ca.cim][ca.klub]</t>
   </si>
@@ -163,12 +163,6 @@
   </si>
   <si>
     <t>[cnum.active;ope=tbs:num]</t>
-  </si>
-  <si>
-    <t>Újra nyitott</t>
-  </si>
-  <si>
-    <t>[cnum.reopened;ope=tbs:num]</t>
   </si>
 </sst>
 </file>
@@ -448,14 +442,14 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="163">
@@ -1018,7 +1012,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R37"/>
+  <dimension ref="A1:R36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1034,18 +1028,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="1" customFormat="1" ht="15" customHeight="1">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
       <c r="K1" s="6"/>
       <c r="L1" s="6"/>
       <c r="M1" s="6"/>
@@ -1101,12 +1095,12 @@
     </row>
     <row r="5" spans="1:18" ht="15" customHeight="1">
       <c r="A5" s="16" t="s">
-        <v>48</v>
+        <v>5</v>
       </c>
       <c r="B5" s="16"/>
       <c r="C5" s="16"/>
       <c r="D5" s="7" t="s">
-        <v>49</v>
+        <v>6</v>
       </c>
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
@@ -1117,12 +1111,12 @@
     </row>
     <row r="6" spans="1:18" ht="15" customHeight="1">
       <c r="A6" s="16" t="s">
-        <v>5</v>
+        <v>46</v>
       </c>
       <c r="B6" s="16"/>
       <c r="C6" s="16"/>
       <c r="D6" s="7" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
@@ -1133,12 +1127,12 @@
     </row>
     <row r="7" spans="1:18" ht="15" customHeight="1">
       <c r="A7" s="16" t="s">
-        <v>46</v>
+        <v>7</v>
       </c>
       <c r="B7" s="16"/>
       <c r="C7" s="16"/>
       <c r="D7" s="7" t="s">
-        <v>47</v>
+        <v>8</v>
       </c>
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
@@ -1149,12 +1143,12 @@
     </row>
     <row r="8" spans="1:18" ht="15" customHeight="1">
       <c r="A8" s="16" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B8" s="16"/>
       <c r="C8" s="16"/>
       <c r="D8" s="7" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
@@ -1164,14 +1158,10 @@
       <c r="J8" s="2"/>
     </row>
     <row r="9" spans="1:18" ht="15" customHeight="1">
-      <c r="A9" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="7" t="s">
-        <v>10</v>
-      </c>
+      <c r="A9" s="2"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="9"/>
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
@@ -1180,10 +1170,14 @@
       <c r="J9" s="2"/>
     </row>
     <row r="10" spans="1:18" ht="15" customHeight="1">
-      <c r="A10" s="2"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="9"/>
+      <c r="A10" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="16"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="7" t="s">
+        <v>27</v>
+      </c>
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
@@ -1193,14 +1187,16 @@
     </row>
     <row r="11" spans="1:18" ht="15" customHeight="1">
       <c r="A11" s="16" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B11" s="16"/>
       <c r="C11" s="16"/>
       <c r="D11" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E11" s="8"/>
+        <v>29</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
       <c r="H11" s="8"/>
@@ -1209,15 +1205,15 @@
     </row>
     <row r="12" spans="1:18" ht="15" customHeight="1">
       <c r="A12" s="16" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B12" s="16"/>
       <c r="C12" s="16"/>
       <c r="D12" s="7" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
@@ -1227,15 +1223,15 @@
     </row>
     <row r="13" spans="1:18" ht="15" customHeight="1">
       <c r="A13" s="16" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B13" s="16"/>
       <c r="C13" s="16"/>
       <c r="D13" s="7" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
@@ -1245,15 +1241,15 @@
     </row>
     <row r="14" spans="1:18" ht="15" customHeight="1">
       <c r="A14" s="16" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B14" s="16"/>
       <c r="C14" s="16"/>
       <c r="D14" s="7" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
@@ -1263,16 +1259,14 @@
     </row>
     <row r="15" spans="1:18" ht="15" customHeight="1">
       <c r="A15" s="16" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B15" s="16"/>
       <c r="C15" s="16"/>
       <c r="D15" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>39</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="E15" s="8"/>
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
       <c r="H15" s="8"/>
@@ -1281,12 +1275,12 @@
     </row>
     <row r="16" spans="1:18" ht="15" customHeight="1">
       <c r="A16" s="16" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B16" s="16"/>
       <c r="C16" s="16"/>
       <c r="D16" s="7" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
@@ -1297,12 +1291,12 @@
     </row>
     <row r="17" spans="1:10" ht="15" customHeight="1">
       <c r="A17" s="16" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B17" s="16"/>
       <c r="C17" s="16"/>
       <c r="D17" s="7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
@@ -1312,14 +1306,10 @@
       <c r="J17" s="2"/>
     </row>
     <row r="18" spans="1:10" ht="15" customHeight="1">
-      <c r="A18" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="B18" s="16"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="7" t="s">
-        <v>45</v>
-      </c>
+      <c r="A18" s="2"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="9"/>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
@@ -1327,40 +1317,44 @@
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
     </row>
-    <row r="19" spans="1:10" ht="15" customHeight="1">
-      <c r="A19" s="2"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-    </row>
-    <row r="20" spans="1:10" ht="30" customHeight="1">
+    <row r="19" spans="1:10" ht="30" customHeight="1">
+      <c r="A19" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
+    </row>
+    <row r="20" spans="1:10" ht="21" customHeight="1">
       <c r="A20" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B20" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="10"/>
-      <c r="I20" s="10"/>
-      <c r="J20" s="10"/>
+        <v>12</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="11"/>
     </row>
     <row r="21" spans="1:10" ht="21" customHeight="1">
       <c r="A21" s="12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C21" s="11"/>
       <c r="D21" s="11"/>
@@ -1372,110 +1366,106 @@
       <c r="J21" s="11"/>
     </row>
     <row r="22" spans="1:10" ht="21" customHeight="1">
-      <c r="A22" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B22" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="11"/>
-      <c r="J22" s="11"/>
+      <c r="A22" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
     </row>
     <row r="23" spans="1:10" ht="21" customHeight="1">
-      <c r="A23" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B23" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="10"/>
-      <c r="I23" s="10"/>
-      <c r="J23" s="10"/>
+      <c r="A23" s="17"/>
+      <c r="B23" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="11"/>
     </row>
     <row r="24" spans="1:10" ht="21" customHeight="1">
-      <c r="A24" s="15"/>
-      <c r="B24" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="11"/>
-      <c r="J24" s="11"/>
+      <c r="A24" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="10"/>
     </row>
     <row r="25" spans="1:10" ht="21" customHeight="1">
-      <c r="A25" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B25" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="10"/>
-      <c r="I25" s="10"/>
-      <c r="J25" s="10"/>
+      <c r="A25" s="17"/>
+      <c r="B25" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11"/>
     </row>
     <row r="26" spans="1:10" ht="21" customHeight="1">
-      <c r="A26" s="15"/>
-      <c r="B26" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="11"/>
-      <c r="I26" s="11"/>
-      <c r="J26" s="11"/>
+      <c r="A26" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="10"/>
+      <c r="J26" s="10"/>
     </row>
     <row r="27" spans="1:10" ht="21" customHeight="1">
-      <c r="A27" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="B27" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="10"/>
-      <c r="I27" s="10"/>
-      <c r="J27" s="10"/>
-    </row>
-    <row r="28" spans="1:10" ht="21" customHeight="1">
-      <c r="A28" s="15"/>
-      <c r="B28" s="14" t="s">
+      <c r="A27" s="17"/>
+      <c r="B27" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="11"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="11"/>
-      <c r="F28" s="11"/>
-      <c r="G28" s="11"/>
-      <c r="H28" s="11"/>
-      <c r="I28" s="11"/>
-      <c r="J28" s="11"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="11"/>
+      <c r="J27" s="11"/>
+    </row>
+    <row r="28" spans="1:10" ht="15" customHeight="1">
+      <c r="A28" s="2"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
     </row>
     <row r="29" spans="1:10" ht="15" customHeight="1">
       <c r="A29" s="2"/>
@@ -1573,39 +1563,26 @@
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
     </row>
-    <row r="37" spans="1:10" ht="15" customHeight="1">
-      <c r="A37" s="2"/>
-      <c r="B37" s="8"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="9"/>
-      <c r="E37" s="8"/>
-      <c r="F37" s="8"/>
-      <c r="G37" s="8"/>
-      <c r="H37" s="8"/>
-      <c r="I37" s="2"/>
-      <c r="J37" s="2"/>
-    </row>
   </sheetData>
-  <mergeCells count="19">
+  <mergeCells count="18">
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A16:C16"/>
     <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A10:C10"/>
     <mergeCell ref="A11:C11"/>
     <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A15:C15"/>
     <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A16:C16"/>
     <mergeCell ref="A14:C14"/>
-    <mergeCell ref="A15:C15"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A5:C5"/>
     <mergeCell ref="A6:C6"/>
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A17:C17"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.8" right="0.2" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
improve catering stat with some additional data field
</commit_message>
<xml_diff>
--- a/src/JCSGYK/AdminBundle/Resources/public/reports/catering_stats.xlsx
+++ b/src/JCSGYK/AdminBundle/Resources/public/reports/catering_stats.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2380" yWindow="1340" windowWidth="46380" windowHeight="26420"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="34420" windowHeight="18340"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>[ca.cim][ca.klub]</t>
   </si>
@@ -42,9 +42,6 @@
     <t>[cnum.all;ope=tbs:num]</t>
   </si>
   <si>
-    <t>Megszűntek</t>
-  </si>
-  <si>
     <t>[cnum.archived;ope=tbs:num]</t>
   </si>
   <si>
@@ -75,12 +72,6 @@
     <t>[age_headers.val;block=tbs:cell]</t>
   </si>
   <si>
-    <t>[age_2.val;block=tbs:cell;ope=tbs:num]</t>
-  </si>
-  <si>
-    <t>[age_1.val;block=tbs:cell;ope=tbs:num]</t>
-  </si>
-  <si>
     <t>[comfort_headers.val;block=tbs:cell]</t>
   </si>
   <si>
@@ -141,9 +132,6 @@
     <t>[inv.payendcli;ope=tbs:num]</t>
   </si>
   <si>
-    <t>Térítési díj bevétel összesen</t>
-  </si>
-  <si>
     <t>[inv.sum]</t>
   </si>
   <si>
@@ -163,6 +151,36 @@
   </si>
   <si>
     <t>[cnum.active;ope=tbs:num]</t>
+  </si>
+  <si>
+    <t>[age_2.val;block=tbs:cell]</t>
+  </si>
+  <si>
+    <t>[age_1.val;block=tbs:cell]</t>
+  </si>
+  <si>
+    <t>Megszűntek (archiváltak)</t>
+  </si>
+  <si>
+    <t>Szünetelők</t>
+  </si>
+  <si>
+    <t>[cnum.paused;ope=tbs:num]</t>
+  </si>
+  <si>
+    <t>Várható térítési díj bevétel összesen</t>
+  </si>
+  <si>
+    <t>Könyvelt térítési díj bevétel összesen</t>
+  </si>
+  <si>
+    <t>[inv.acc]</t>
+  </si>
+  <si>
+    <t>Térítési díj elmaradás összesen</t>
+  </si>
+  <si>
+    <t>[inv.def]</t>
   </si>
 </sst>
 </file>
@@ -217,7 +235,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -240,8 +258,45 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="163">
+  <cellStyleXfs count="181">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -405,8 +460,26 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -451,8 +524,20 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="163">
+  <cellStyles count="181">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -534,6 +619,15 @@
     <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -615,6 +709,15 @@
     <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1012,10 +1115,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R36"/>
+  <dimension ref="A1:R39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.7109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
@@ -1111,12 +1214,12 @@
     </row>
     <row r="6" spans="1:18" ht="15" customHeight="1">
       <c r="A6" s="16" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B6" s="16"/>
       <c r="C6" s="16"/>
       <c r="D6" s="7" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
@@ -1127,12 +1230,12 @@
     </row>
     <row r="7" spans="1:18" ht="15" customHeight="1">
       <c r="A7" s="16" t="s">
-        <v>7</v>
+        <v>47</v>
       </c>
       <c r="B7" s="16"/>
       <c r="C7" s="16"/>
       <c r="D7" s="7" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
@@ -1143,12 +1246,12 @@
     </row>
     <row r="8" spans="1:18" ht="15" customHeight="1">
       <c r="A8" s="16" t="s">
-        <v>9</v>
+        <v>46</v>
       </c>
       <c r="B8" s="16"/>
       <c r="C8" s="16"/>
       <c r="D8" s="7" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
@@ -1158,10 +1261,14 @@
       <c r="J8" s="2"/>
     </row>
     <row r="9" spans="1:18" ht="15" customHeight="1">
-      <c r="A9" s="2"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="9"/>
+      <c r="A9" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="7" t="s">
+        <v>9</v>
+      </c>
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
@@ -1170,14 +1277,10 @@
       <c r="J9" s="2"/>
     </row>
     <row r="10" spans="1:18" ht="15" customHeight="1">
-      <c r="A10" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="7" t="s">
-        <v>27</v>
-      </c>
+      <c r="A10" s="2"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="9"/>
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
@@ -1187,16 +1290,14 @@
     </row>
     <row r="11" spans="1:18" ht="15" customHeight="1">
       <c r="A11" s="16" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B11" s="16"/>
       <c r="C11" s="16"/>
       <c r="D11" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>30</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="E11" s="8"/>
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
       <c r="H11" s="8"/>
@@ -1205,15 +1306,15 @@
     </row>
     <row r="12" spans="1:18" ht="15" customHeight="1">
       <c r="A12" s="16" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B12" s="16"/>
       <c r="C12" s="16"/>
       <c r="D12" s="7" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
@@ -1223,15 +1324,15 @@
     </row>
     <row r="13" spans="1:18" ht="15" customHeight="1">
       <c r="A13" s="16" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B13" s="16"/>
       <c r="C13" s="16"/>
       <c r="D13" s="7" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
@@ -1241,15 +1342,15 @@
     </row>
     <row r="14" spans="1:18" ht="15" customHeight="1">
       <c r="A14" s="16" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B14" s="16"/>
       <c r="C14" s="16"/>
       <c r="D14" s="7" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
@@ -1259,14 +1360,16 @@
     </row>
     <row r="15" spans="1:18" ht="15" customHeight="1">
       <c r="A15" s="16" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B15" s="16"/>
       <c r="C15" s="16"/>
       <c r="D15" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E15" s="8"/>
+        <v>35</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>36</v>
+      </c>
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
       <c r="H15" s="8"/>
@@ -1275,12 +1378,12 @@
     </row>
     <row r="16" spans="1:18" ht="15" customHeight="1">
       <c r="A16" s="16" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="B16" s="16"/>
       <c r="C16" s="16"/>
       <c r="D16" s="7" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
@@ -1290,13 +1393,13 @@
       <c r="J16" s="2"/>
     </row>
     <row r="17" spans="1:10" ht="15" customHeight="1">
-      <c r="A17" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="B17" s="16"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="7" t="s">
-        <v>45</v>
+      <c r="A17" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" s="20"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="18" t="s">
+        <v>51</v>
       </c>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
@@ -1306,10 +1409,14 @@
       <c r="J17" s="2"/>
     </row>
     <row r="18" spans="1:10" ht="15" customHeight="1">
-      <c r="A18" s="2"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="9"/>
+      <c r="A18" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" s="20"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="18" t="s">
+        <v>53</v>
+      </c>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
@@ -1317,60 +1424,56 @@
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
     </row>
-    <row r="19" spans="1:10" ht="30" customHeight="1">
-      <c r="A19" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B19" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="10"/>
-      <c r="J19" s="10"/>
-    </row>
-    <row r="20" spans="1:10" ht="21" customHeight="1">
-      <c r="A20" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B20" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
-      <c r="J20" s="11"/>
-    </row>
-    <row r="21" spans="1:10" ht="21" customHeight="1">
-      <c r="A21" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B21" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="11"/>
-      <c r="J21" s="11"/>
-    </row>
-    <row r="22" spans="1:10" ht="21" customHeight="1">
-      <c r="A22" s="17" t="s">
-        <v>14</v>
+    <row r="19" spans="1:10" ht="15" customHeight="1">
+      <c r="A19" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="16"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+    </row>
+    <row r="20" spans="1:10" ht="15" customHeight="1">
+      <c r="A20" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="16"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+    </row>
+    <row r="21" spans="1:10" ht="15" customHeight="1">
+      <c r="A21" s="2"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+    </row>
+    <row r="22" spans="1:10" ht="30" customHeight="1">
+      <c r="A22" s="12" t="s">
+        <v>10</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C22" s="10"/>
       <c r="D22" s="10"/>
@@ -1382,9 +1485,11 @@
       <c r="J22" s="10"/>
     </row>
     <row r="23" spans="1:10" ht="21" customHeight="1">
-      <c r="A23" s="17"/>
+      <c r="A23" s="12" t="s">
+        <v>11</v>
+      </c>
       <c r="B23" s="14" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="C23" s="11"/>
       <c r="D23" s="11"/>
@@ -1396,100 +1501,110 @@
       <c r="J23" s="11"/>
     </row>
     <row r="24" spans="1:10" ht="21" customHeight="1">
-      <c r="A24" s="17" t="s">
+      <c r="A24" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="11"/>
+    </row>
+    <row r="25" spans="1:10" ht="21" customHeight="1">
+      <c r="A25" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="10"/>
+    </row>
+    <row r="26" spans="1:10" ht="21" customHeight="1">
+      <c r="A26" s="17"/>
+      <c r="B26" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="11"/>
+    </row>
+    <row r="27" spans="1:10" ht="21" customHeight="1">
+      <c r="A27" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="10"/>
+    </row>
+    <row r="28" spans="1:10" ht="21" customHeight="1">
+      <c r="A28" s="17"/>
+      <c r="B28" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="11"/>
+      <c r="J28" s="11"/>
+    </row>
+    <row r="29" spans="1:10" ht="21" customHeight="1">
+      <c r="A29" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="B24" s="13" t="s">
+      <c r="B29" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="10"/>
+      <c r="I29" s="10"/>
+      <c r="J29" s="10"/>
+    </row>
+    <row r="30" spans="1:10" ht="21" customHeight="1">
+      <c r="A30" s="17"/>
+      <c r="B30" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="10"/>
-      <c r="I24" s="10"/>
-      <c r="J24" s="10"/>
-    </row>
-    <row r="25" spans="1:10" ht="21" customHeight="1">
-      <c r="A25" s="17"/>
-      <c r="B25" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="C25" s="11"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="11"/>
-      <c r="J25" s="11"/>
-    </row>
-    <row r="26" spans="1:10" ht="21" customHeight="1">
-      <c r="A26" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="B26" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="C26" s="10"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="10"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="10"/>
-      <c r="I26" s="10"/>
-      <c r="J26" s="10"/>
-    </row>
-    <row r="27" spans="1:10" ht="21" customHeight="1">
-      <c r="A27" s="17"/>
-      <c r="B27" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="C27" s="11"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="11"/>
-      <c r="I27" s="11"/>
-      <c r="J27" s="11"/>
-    </row>
-    <row r="28" spans="1:10" ht="15" customHeight="1">
-      <c r="A28" s="2"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
-      <c r="I28" s="2"/>
-      <c r="J28" s="2"/>
-    </row>
-    <row r="29" spans="1:10" ht="15" customHeight="1">
-      <c r="A29" s="2"/>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="2"/>
-      <c r="J29" s="2"/>
-    </row>
-    <row r="30" spans="1:10" ht="15" customHeight="1">
-      <c r="A30" s="2"/>
-      <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="8"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="8"/>
-      <c r="H30" s="8"/>
-      <c r="I30" s="2"/>
-      <c r="J30" s="2"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="11"/>
+      <c r="J30" s="11"/>
     </row>
     <row r="31" spans="1:10" ht="15" customHeight="1">
       <c r="A31" s="2"/>
@@ -1563,25 +1678,64 @@
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
     </row>
+    <row r="37" spans="1:10" ht="15" customHeight="1">
+      <c r="A37" s="2"/>
+      <c r="B37" s="8"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="8"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
+    </row>
+    <row r="38" spans="1:10" ht="15" customHeight="1">
+      <c r="A38" s="2"/>
+      <c r="B38" s="8"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="8"/>
+      <c r="H38" s="8"/>
+      <c r="I38" s="2"/>
+      <c r="J38" s="2"/>
+    </row>
+    <row r="39" spans="1:10" ht="15" customHeight="1">
+      <c r="A39" s="2"/>
+      <c r="B39" s="8"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="8"/>
+      <c r="G39" s="8"/>
+      <c r="H39" s="8"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
+    </row>
   </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="A26:A27"/>
+  <mergeCells count="21">
     <mergeCell ref="A17:C17"/>
-    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A19:C19"/>
     <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A10:C10"/>
     <mergeCell ref="A11:C11"/>
     <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A14:C14"/>
     <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A14:C14"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="A4:C4"/>
     <mergeCell ref="A5:C5"/>
     <mergeCell ref="A6:C6"/>
     <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A9:C9"/>
     <mergeCell ref="A8:C8"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
replace opentbs with phpexcel to generate xlsx statistic documents
</commit_message>
<xml_diff>
--- a/src/JCSGYK/AdminBundle/Resources/public/reports/catering_stats.xlsx
+++ b/src/JCSGYK/AdminBundle/Resources/public/reports/catering_stats.xlsx
@@ -27,30 +27,15 @@
     <t>Létszám hónap 1-én</t>
   </si>
   <si>
-    <t>[cnum.start;ope=tbs:num]</t>
-  </si>
-  <si>
     <t>Új felvétel</t>
   </si>
   <si>
-    <t>[cnum.new;ope=tbs:num]</t>
-  </si>
-  <si>
     <t>Teljes havi létszám</t>
   </si>
   <si>
-    <t>[cnum.all;ope=tbs:num]</t>
-  </si>
-  <si>
-    <t>[cnum.archived;ope=tbs:num]</t>
-  </si>
-  <si>
     <t>Létszám hónap végén</t>
   </si>
   <si>
-    <t>[cnum.end;ope=tbs:num]</t>
-  </si>
-  <si>
     <t>Kor szerinti megoszlás</t>
   </si>
   <si>
@@ -69,69 +54,21 @@
     <t>Lakásban tartózkodás jogcíme</t>
   </si>
   <si>
-    <t>[age_headers.val;block=tbs:cell]</t>
-  </si>
-  <si>
-    <t>[comfort_headers.val;block=tbs:cell]</t>
-  </si>
-  <si>
-    <t>[comfort.val;block=tbs:cell;ope=tbs:num]</t>
-  </si>
-  <si>
-    <t>[income_headers.val;block=tbs:cell]</t>
-  </si>
-  <si>
-    <t>[income.val;block=tbs:cell;ope=tbs:num]</t>
-  </si>
-  <si>
-    <t>[ownership_headers.val;block=tbs:cell]</t>
-  </si>
-  <si>
-    <t>[ownership.val;block=tbs:cell;ope=tbs:num]</t>
-  </si>
-  <si>
     <t>Étkezési napok száma</t>
   </si>
   <si>
-    <t>[inv.days;ope=tbs:num]</t>
-  </si>
-  <si>
     <t>TM ebéd H-P adag / fő</t>
   </si>
   <si>
-    <t>[inv.discweek;ope=tbs:num]</t>
-  </si>
-  <si>
-    <t>[inv.discweekcli;ope=tbs:num]</t>
-  </si>
-  <si>
     <t>TM ebéd hétvége adag / fő</t>
   </si>
   <si>
-    <t>[inv.discendcli;ope=tbs:num]</t>
-  </si>
-  <si>
-    <t>[inv.discend;ope=tbs:num]</t>
-  </si>
-  <si>
     <t>Fizetős ebéd H-P adag / fő</t>
   </si>
   <si>
     <t>Fizetős ebéd hétvége adag / fő</t>
   </si>
   <si>
-    <t>[inv.payweek;ope=tbs:num]</t>
-  </si>
-  <si>
-    <t>[inv.payweekcli;ope=tbs:num]</t>
-  </si>
-  <si>
-    <t>[inv.payend;ope=tbs:num]</t>
-  </si>
-  <si>
-    <t>[inv.payendcli;ope=tbs:num]</t>
-  </si>
-  <si>
     <t>[inv.sum]</t>
   </si>
   <si>
@@ -141,33 +78,15 @@
     <t>Étkezők száma FÉRFI</t>
   </si>
   <si>
-    <t>[cnum.woman;ope=tbs:num]</t>
-  </si>
-  <si>
-    <t>[cnum.man;ope=tbs:num]</t>
-  </si>
-  <si>
     <t>Aktív ellátottak száma</t>
   </si>
   <si>
-    <t>[cnum.active;ope=tbs:num]</t>
-  </si>
-  <si>
-    <t>[age_2.val;block=tbs:cell]</t>
-  </si>
-  <si>
-    <t>[age_1.val;block=tbs:cell]</t>
-  </si>
-  <si>
     <t>Megszűntek (archiváltak)</t>
   </si>
   <si>
     <t>Szünetelők</t>
   </si>
   <si>
-    <t>[cnum.paused;ope=tbs:num]</t>
-  </si>
-  <si>
     <t>Várható térítési díj bevétel összesen</t>
   </si>
   <si>
@@ -181,13 +100,94 @@
   </si>
   <si>
     <t>[inv.def]</t>
+  </si>
+  <si>
+    <t>[age_headers]</t>
+  </si>
+  <si>
+    <t>[age_2]</t>
+  </si>
+  <si>
+    <t>[age_1]</t>
+  </si>
+  <si>
+    <t>[comfort_headers]</t>
+  </si>
+  <si>
+    <t>[comfort]</t>
+  </si>
+  <si>
+    <t>[income_headers]</t>
+  </si>
+  <si>
+    <t>[income]</t>
+  </si>
+  <si>
+    <t>[ownership_headers]</t>
+  </si>
+  <si>
+    <t>[ownership]</t>
+  </si>
+  <si>
+    <t>[cnum.start]</t>
+  </si>
+  <si>
+    <t>[cnum.new]</t>
+  </si>
+  <si>
+    <t>[cnum.all]</t>
+  </si>
+  <si>
+    <t>[cnum.active]</t>
+  </si>
+  <si>
+    <t>[cnum.paused]</t>
+  </si>
+  <si>
+    <t>[cnum.archived]</t>
+  </si>
+  <si>
+    <t>[cnum.end]</t>
+  </si>
+  <si>
+    <t>[inv.days]</t>
+  </si>
+  <si>
+    <t>[inv.discweek]</t>
+  </si>
+  <si>
+    <t>[inv.discweekcli]</t>
+  </si>
+  <si>
+    <t>[inv.discend]</t>
+  </si>
+  <si>
+    <t>[inv.discendcli]</t>
+  </si>
+  <si>
+    <t>[inv.payweek]</t>
+  </si>
+  <si>
+    <t>[inv.payweekcli]</t>
+  </si>
+  <si>
+    <t>[inv.payend]</t>
+  </si>
+  <si>
+    <t>[inv.payendcli]</t>
+  </si>
+  <si>
+    <t>[cnum.woman]</t>
+  </si>
+  <si>
+    <t>[cnum.man]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial CE"/>
@@ -226,16 +226,27 @@
       <sz val="11"/>
       <name val="Arial CE"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Arial CE"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -295,6 +306,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="181">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -479,7 +516,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -491,9 +528,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -506,35 +540,44 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="181">
@@ -1118,7 +1161,7 @@
   <dimension ref="A1:R39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.7109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
@@ -1131,18 +1174,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="1" customFormat="1" ht="15" customHeight="1">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
       <c r="K1" s="6"/>
       <c r="L1" s="6"/>
       <c r="M1" s="6"/>
@@ -1154,342 +1197,342 @@
     </row>
     <row r="2" spans="1:18" ht="15" customHeight="1">
       <c r="A2" s="2"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
     </row>
     <row r="3" spans="1:18" ht="15" customHeight="1">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
     </row>
     <row r="4" spans="1:18" ht="15" customHeight="1">
-      <c r="A4" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
+      <c r="A4" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
     </row>
     <row r="5" spans="1:18" ht="15" customHeight="1">
-      <c r="A5" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
+      <c r="A5" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
     </row>
     <row r="6" spans="1:18" ht="15" customHeight="1">
-      <c r="A6" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
+      <c r="A6" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
     </row>
     <row r="7" spans="1:18" ht="15" customHeight="1">
-      <c r="A7" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
+      <c r="A7" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
     </row>
     <row r="8" spans="1:18" ht="15" customHeight="1">
-      <c r="A8" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
+      <c r="A8" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
     </row>
     <row r="9" spans="1:18" ht="15" customHeight="1">
-      <c r="A9" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
+      <c r="A9" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
     </row>
     <row r="10" spans="1:18" ht="15" customHeight="1">
       <c r="A10" s="2"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
     </row>
     <row r="11" spans="1:18" ht="15" customHeight="1">
-      <c r="A11" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" s="16"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
+      <c r="A11" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
     </row>
     <row r="12" spans="1:18" ht="15" customHeight="1">
-      <c r="A12" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="16"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
+      <c r="A12" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
     </row>
     <row r="13" spans="1:18" ht="15" customHeight="1">
-      <c r="A13" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13" s="16"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
+      <c r="A13" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
     </row>
     <row r="14" spans="1:18" ht="15" customHeight="1">
-      <c r="A14" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="B14" s="16"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
+      <c r="A14" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
     </row>
     <row r="15" spans="1:18" ht="15" customHeight="1">
-      <c r="A15" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="B15" s="16"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
+      <c r="A15" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
     </row>
     <row r="16" spans="1:18" ht="15" customHeight="1">
-      <c r="A16" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
+      <c r="A16" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="15"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
     </row>
     <row r="17" spans="1:10" ht="15" customHeight="1">
-      <c r="A17" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="B17" s="20"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
+      <c r="A17" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="17"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
     </row>
     <row r="18" spans="1:10" ht="15" customHeight="1">
-      <c r="A18" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="B18" s="20"/>
-      <c r="C18" s="21"/>
-      <c r="D18" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
+      <c r="A18" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="17"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
     </row>
     <row r="19" spans="1:10" ht="15" customHeight="1">
-      <c r="A19" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="B19" s="16"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
+      <c r="A19" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="15"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
     </row>
     <row r="20" spans="1:10" ht="15" customHeight="1">
-      <c r="A20" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="B20" s="16"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
+      <c r="A20" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
     </row>
     <row r="21" spans="1:10" ht="15" customHeight="1">
       <c r="A21" s="2"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
     </row>
     <row r="22" spans="1:10" ht="30" customHeight="1">
-      <c r="A22" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B22" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="10"/>
-      <c r="I22" s="10"/>
-      <c r="J22" s="10"/>
+      <c r="A22" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="20"/>
+      <c r="I22" s="20"/>
+      <c r="J22" s="20"/>
     </row>
     <row r="23" spans="1:10" ht="21" customHeight="1">
-      <c r="A23" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B23" s="14" t="s">
-        <v>44</v>
+      <c r="A23" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>28</v>
       </c>
       <c r="C23" s="11"/>
       <c r="D23" s="11"/>
@@ -1501,11 +1544,11 @@
       <c r="J23" s="11"/>
     </row>
     <row r="24" spans="1:10" ht="21" customHeight="1">
-      <c r="A24" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B24" s="14" t="s">
-        <v>45</v>
+      <c r="A24" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>29</v>
       </c>
       <c r="C24" s="11"/>
       <c r="D24" s="11"/>
@@ -1517,212 +1560,205 @@
       <c r="J24" s="11"/>
     </row>
     <row r="25" spans="1:10" ht="21" customHeight="1">
-      <c r="A25" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="B25" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="10"/>
-      <c r="I25" s="10"/>
-      <c r="J25" s="10"/>
+      <c r="A25" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="9"/>
     </row>
     <row r="26" spans="1:10" ht="21" customHeight="1">
-      <c r="A26" s="17"/>
-      <c r="B26" s="14" t="s">
-        <v>18</v>
+      <c r="A26" s="23"/>
+      <c r="B26" s="11" t="s">
+        <v>31</v>
       </c>
       <c r="C26" s="11"/>
       <c r="D26" s="11"/>
       <c r="E26" s="11"/>
       <c r="F26" s="11"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="11"/>
-      <c r="I26" s="11"/>
-      <c r="J26" s="11"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="10"/>
+      <c r="J26" s="10"/>
     </row>
     <row r="27" spans="1:10" ht="21" customHeight="1">
-      <c r="A27" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="B27" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="10"/>
-      <c r="I27" s="10"/>
-      <c r="J27" s="10"/>
+      <c r="A27" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="B27" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="C27" s="20"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="9"/>
     </row>
     <row r="28" spans="1:10" ht="21" customHeight="1">
-      <c r="A28" s="17"/>
-      <c r="B28" s="14" t="s">
-        <v>20</v>
+      <c r="A28" s="23"/>
+      <c r="B28" s="11" t="s">
+        <v>33</v>
       </c>
       <c r="C28" s="11"/>
       <c r="D28" s="11"/>
       <c r="E28" s="11"/>
       <c r="F28" s="11"/>
-      <c r="G28" s="11"/>
-      <c r="H28" s="11"/>
-      <c r="I28" s="11"/>
-      <c r="J28" s="11"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="10"/>
+      <c r="J28" s="10"/>
     </row>
     <row r="29" spans="1:10" ht="21" customHeight="1">
-      <c r="A29" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="B29" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="10"/>
-      <c r="G29" s="10"/>
-      <c r="H29" s="10"/>
-      <c r="I29" s="10"/>
-      <c r="J29" s="10"/>
+      <c r="A29" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="C29" s="20"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="9"/>
     </row>
     <row r="30" spans="1:10" ht="21" customHeight="1">
-      <c r="A30" s="17"/>
-      <c r="B30" s="14" t="s">
-        <v>22</v>
+      <c r="A30" s="23"/>
+      <c r="B30" s="11" t="s">
+        <v>35</v>
       </c>
       <c r="C30" s="11"/>
       <c r="D30" s="11"/>
       <c r="E30" s="11"/>
       <c r="F30" s="11"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="11"/>
-      <c r="I30" s="11"/>
-      <c r="J30" s="11"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="10"/>
+      <c r="J30" s="10"/>
     </row>
     <row r="31" spans="1:10" ht="15" customHeight="1">
       <c r="A31" s="2"/>
-      <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="8"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="8"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="7"/>
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
     </row>
     <row r="32" spans="1:10" ht="15" customHeight="1">
       <c r="A32" s="2"/>
-      <c r="B32" s="8"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="8"/>
-      <c r="F32" s="8"/>
-      <c r="G32" s="8"/>
-      <c r="H32" s="8"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="7"/>
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
     </row>
     <row r="33" spans="1:10" ht="15" customHeight="1">
       <c r="A33" s="2"/>
-      <c r="B33" s="8"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="8"/>
-      <c r="G33" s="8"/>
-      <c r="H33" s="8"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
     </row>
     <row r="34" spans="1:10" ht="15" customHeight="1">
       <c r="A34" s="2"/>
-      <c r="B34" s="8"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="8"/>
-      <c r="F34" s="8"/>
-      <c r="G34" s="8"/>
-      <c r="H34" s="8"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7"/>
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
     </row>
     <row r="35" spans="1:10" ht="15" customHeight="1">
       <c r="A35" s="2"/>
-      <c r="B35" s="8"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="8"/>
-      <c r="F35" s="8"/>
-      <c r="G35" s="8"/>
-      <c r="H35" s="8"/>
+      <c r="B35" s="7"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="8"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
+      <c r="H35" s="7"/>
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
     </row>
     <row r="36" spans="1:10" ht="15" customHeight="1">
       <c r="A36" s="2"/>
-      <c r="B36" s="8"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="9"/>
-      <c r="E36" s="8"/>
-      <c r="F36" s="8"/>
-      <c r="G36" s="8"/>
-      <c r="H36" s="8"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="7"/>
+      <c r="H36" s="7"/>
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
     </row>
     <row r="37" spans="1:10" ht="15" customHeight="1">
       <c r="A37" s="2"/>
-      <c r="B37" s="8"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="9"/>
-      <c r="E37" s="8"/>
-      <c r="F37" s="8"/>
-      <c r="G37" s="8"/>
-      <c r="H37" s="8"/>
+      <c r="B37" s="7"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7"/>
+      <c r="G37" s="7"/>
+      <c r="H37" s="7"/>
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
     </row>
     <row r="38" spans="1:10" ht="15" customHeight="1">
       <c r="A38" s="2"/>
-      <c r="B38" s="8"/>
-      <c r="C38" s="8"/>
-      <c r="D38" s="9"/>
-      <c r="E38" s="8"/>
-      <c r="F38" s="8"/>
-      <c r="G38" s="8"/>
-      <c r="H38" s="8"/>
+      <c r="B38" s="7"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="7"/>
+      <c r="H38" s="7"/>
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
     </row>
     <row r="39" spans="1:10" ht="15" customHeight="1">
       <c r="A39" s="2"/>
-      <c r="B39" s="8"/>
-      <c r="C39" s="8"/>
-      <c r="D39" s="9"/>
-      <c r="E39" s="8"/>
-      <c r="F39" s="8"/>
-      <c r="G39" s="8"/>
-      <c r="H39" s="8"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="7"/>
+      <c r="G39" s="7"/>
+      <c r="H39" s="7"/>
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="A19:C19"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A11:C11"/>
     <mergeCell ref="A12:C12"/>
@@ -1737,6 +1773,13 @@
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="A9:C9"/>
     <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A19:C19"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.8" right="0.2" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>